<commit_message>
Minor Change in Metadata
</commit_message>
<xml_diff>
--- a/Data/IHBS/RFiles/Data/MetaDataN.xlsx
+++ b/Data/IHBS/RFiles/Data/MetaDataN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dashboard\to github\IRHEIS-master\IRHEIS-master\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1B77F7-EC8E-4944-8D5F-F425802C9B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8C2143-F352-4A5F-B687-6A9336140EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="858" firstSheet="49" activeTab="49" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12360" yWindow="4776" windowWidth="23040" windowHeight="6000" tabRatio="858" firstSheet="27" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FoodGroupTablesNew (3)" sheetId="1252" r:id="rId1"/>
@@ -2664,8 +2664,8 @@
   <sheetPr codeName="Sheet117"/>
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:O28"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7916,7 +7916,7 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M28"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9953,7 +9953,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15284,8 +15284,8 @@
   <sheetPr codeName="Sheet42"/>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15963,8 +15963,8 @@
   <sheetPr codeName="Sheet49"/>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" activeCellId="1" sqref="L1:L1048576 M1:M1048576"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16636,8 +16636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5416D23A-F71D-47F7-81CD-1BC698BD5FD6}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" activeCellId="1" sqref="L1:L1048576 M1:M1048576"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17309,8 +17309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5045499-F41D-4521-9486-563370E50088}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18864,8 +18864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04762473-50DF-4A04-9886-CE042758A0D7}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19256,10 +19256,10 @@
         <v>28</v>
       </c>
       <c r="C34">
-        <v>62223</v>
+        <v>62322</v>
       </c>
       <c r="D34">
-        <v>62226</v>
+        <v>62348</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -19291,10 +19291,10 @@
         <v>28</v>
       </c>
       <c r="C35">
-        <v>62223</v>
+        <v>62322</v>
       </c>
       <c r="D35">
-        <v>62226</v>
+        <v>62348</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -19326,10 +19326,10 @@
         <v>28</v>
       </c>
       <c r="C36">
-        <v>62223</v>
+        <v>62322</v>
       </c>
       <c r="D36">
-        <v>62226</v>
+        <v>62348</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -19361,10 +19361,10 @@
         <v>28</v>
       </c>
       <c r="C37">
-        <v>62223</v>
+        <v>62322</v>
       </c>
       <c r="D37">
-        <v>62226</v>
+        <v>62348</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -19396,10 +19396,10 @@
         <v>28</v>
       </c>
       <c r="C38">
-        <v>62223</v>
+        <v>62322</v>
       </c>
       <c r="D38">
-        <v>62226</v>
+        <v>62348</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -19431,10 +19431,10 @@
         <v>28</v>
       </c>
       <c r="C39">
-        <v>62223</v>
+        <v>62322</v>
       </c>
       <c r="D39">
-        <v>62226</v>
+        <v>62348</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -19466,10 +19466,10 @@
         <v>28</v>
       </c>
       <c r="C40">
-        <v>62223</v>
+        <v>62322</v>
       </c>
       <c r="D40">
-        <v>62226</v>
+        <v>62348</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -19501,10 +19501,10 @@
         <v>28</v>
       </c>
       <c r="C41">
-        <v>62223</v>
+        <v>62322</v>
       </c>
       <c r="D41">
-        <v>62226</v>
+        <v>62348</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -25656,7 +25656,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:O8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33752,7 +33752,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:O28"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34630,7 +34630,7 @@
   <sheetPr codeName="Sheet55"/>
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>

</xml_diff>